<commit_message>
Edit receipt: Fixed a bug while editing the related invoice.
Backend Tests: Added DRY functions and moved common util files to project level directory.

Receipt list: Added backend tests

Front-end tests: Now searching tests don't raise false errors (hopefully) and run faster.
</commit_message>
<xml_diff>
--- a/erp/tests/files/receivables/receipt_multiple.xlsx
+++ b/erp/tests/files/receivables/receipt_multiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp Pavilion\Documents\Tut y cursos\CS50 - Intro Web Programming\Final Project\receivables\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758EA439-52E3-4C2E-9886-104441730795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF9F158-9C23-4439-A13D-8771D7D5D704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -909,7 +909,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <v>1209</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1091,7 +1091,7 @@
         <v>20361382480</v>
       </c>
       <c r="E6">
-        <v>20999999999</v>
+        <v>99999999999</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>

</xml_diff>